<commit_message>
Installers Version: 1.1.104104 - May 19, 2025
</commit_message>
<xml_diff>
--- a/tutorials/first-document.xlsx
+++ b/tutorials/first-document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevor/repositories/darty/darty-ai-samples/tutorials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88D0E4C-9CA8-CD40-A28F-D673B1740EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E00F50D-FB06-7947-8F6F-0EB2C434DB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6380" yWindow="3300" windowWidth="26840" windowHeight="15940" xr2:uid="{7B82346F-C8FD-1641-B364-70FA67E09AEF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>appearance</t>
   </si>
@@ -44,12 +44,6 @@
     <t>transform</t>
   </si>
   <si>
-    <t>strokeColor</t>
-  </si>
-  <si>
-    <t>strokeWidth</t>
-  </si>
-  <si>
     <t>fillColor</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Violet Blue</t>
   </si>
   <si>
-    <t>square</t>
-  </si>
-  <si>
     <t>anchorPoint</t>
   </si>
   <si>
@@ -132,6 +123,39 @@
   </si>
   <si>
     <t>155, 128, 200</t>
+  </si>
+  <si>
+    <t>stroke[2]Color</t>
+  </si>
+  <si>
+    <t>stroke[2]Width</t>
+  </si>
+  <si>
+    <t>!black</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>234 50 20</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>100, 0 50 0</t>
+  </si>
+  <si>
+    <t>tan</t>
+  </si>
+  <si>
+    <t>fillColor: red</t>
+  </si>
+  <si>
+    <t>#0f0</t>
+  </si>
+  <si>
+    <t>2nd stroke color</t>
   </si>
 </sst>
 </file>
@@ -503,15 +527,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D4FFBE-891C-B44F-A69D-859414BE0ECC}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -519,50 +543,62 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -571,29 +607,32 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -605,15 +644,18 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -622,55 +664,68 @@
         <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>